<commit_message>
Añadida función para cargar automáticamente los ID de Sesión de Maxiconsumo y Andina
</commit_message>
<xml_diff>
--- a/archivos/andina-ACTUALIZADO.xlsx
+++ b/archivos/andina-ACTUALIZADO.xlsx
@@ -2521,7 +2521,7 @@
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 991,65</t>
         </is>
       </c>
     </row>
@@ -2829,7 +2829,7 @@
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr">
         <is>
-          <t>$ 2.809,83</t>
+          <t>$ 2.479,26</t>
         </is>
       </c>
     </row>
@@ -2857,7 +2857,7 @@
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr">
         <is>
-          <t>$ 2.809,83</t>
+          <t>$ 2.479,26</t>
         </is>
       </c>
     </row>
@@ -3781,7 +3781,7 @@
       <c r="E120" t="inlineStr"/>
       <c r="F120" t="inlineStr">
         <is>
-          <t>$ 1.652,81</t>
+          <t>$ 1.818,10</t>
         </is>
       </c>
     </row>
@@ -3809,7 +3809,7 @@
       <c r="E121" t="inlineStr"/>
       <c r="F121" t="inlineStr">
         <is>
-          <t>$ 1.652,81</t>
+          <t>$ 1.818,10</t>
         </is>
       </c>
     </row>
@@ -4397,7 +4397,7 @@
       <c r="E142" t="inlineStr"/>
       <c r="F142" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 909,01</t>
         </is>
       </c>
     </row>
@@ -4621,7 +4621,7 @@
       <c r="E150" t="inlineStr"/>
       <c r="F150" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 512,31</t>
         </is>
       </c>
     </row>
@@ -5209,7 +5209,7 @@
       <c r="E171" t="inlineStr"/>
       <c r="F171" t="inlineStr">
         <is>
-          <t>$ 805,33</t>
+          <t>$ 927,51</t>
         </is>
       </c>
     </row>
@@ -5489,7 +5489,7 @@
       <c r="E181" t="inlineStr"/>
       <c r="F181" t="inlineStr">
         <is>
-          <t>$ 479,55</t>
+          <t>$ 633,39</t>
         </is>
       </c>
     </row>
@@ -5629,7 +5629,7 @@
       <c r="E186" t="inlineStr"/>
       <c r="F186" t="inlineStr">
         <is>
-          <t>$ 696,74</t>
+          <t>$ 687,69</t>
         </is>
       </c>
     </row>
@@ -6693,7 +6693,7 @@
       <c r="E224" t="inlineStr"/>
       <c r="F224" t="inlineStr">
         <is>
-          <t>$ 678,64</t>
+          <t>$ 746,51</t>
         </is>
       </c>
     </row>
@@ -7841,7 +7841,7 @@
       <c r="E265" t="inlineStr"/>
       <c r="F265" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 2.272,64</t>
         </is>
       </c>
     </row>
@@ -7869,7 +7869,7 @@
       <c r="E266" t="inlineStr"/>
       <c r="F266" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 2.272,64</t>
         </is>
       </c>
     </row>
@@ -7897,7 +7897,7 @@
       <c r="E267" t="inlineStr"/>
       <c r="F267" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 2.272,64</t>
         </is>
       </c>
     </row>
@@ -8205,7 +8205,7 @@
       <c r="E278" t="inlineStr"/>
       <c r="F278" t="inlineStr">
         <is>
-          <t>$ 313,97</t>
+          <t>$ 330,50</t>
         </is>
       </c>
     </row>
@@ -8289,7 +8289,7 @@
       <c r="E281" t="inlineStr"/>
       <c r="F281" t="inlineStr">
         <is>
-          <t>$ 313,97</t>
+          <t>$ 330,50</t>
         </is>
       </c>
     </row>
@@ -8401,7 +8401,7 @@
       <c r="E285" t="inlineStr"/>
       <c r="F285" t="inlineStr">
         <is>
-          <t>$ 904,88</t>
+          <t>$ 1.284,98</t>
         </is>
       </c>
     </row>
@@ -8429,7 +8429,7 @@
       <c r="E286" t="inlineStr"/>
       <c r="F286" t="inlineStr">
         <is>
-          <t>$ 1.058,73</t>
+          <t>$ 1.173,19</t>
         </is>
       </c>
     </row>
@@ -8457,7 +8457,7 @@
       <c r="E287" t="inlineStr"/>
       <c r="F287" t="inlineStr">
         <is>
-          <t>$ 814,38</t>
+          <t>$ 1.221,63</t>
         </is>
       </c>
     </row>
@@ -8653,7 +8653,7 @@
       <c r="E294" t="inlineStr"/>
       <c r="F294" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 454,46</t>
         </is>
       </c>
     </row>
@@ -8709,7 +8709,7 @@
       <c r="E296" t="inlineStr"/>
       <c r="F296" t="inlineStr">
         <is>
-          <t>$ 991,65</t>
+          <t>$ 330,49</t>
         </is>
       </c>
     </row>
@@ -10697,7 +10697,7 @@
       <c r="E367" t="inlineStr"/>
       <c r="F367" t="inlineStr">
         <is>
-          <t>$ 1.818,09</t>
+          <t>$ 1.652,81</t>
         </is>
       </c>
     </row>
@@ -10781,7 +10781,7 @@
       <c r="E370" t="inlineStr"/>
       <c r="F370" t="inlineStr">
         <is>
-          <t>$ 1.032,97</t>
+          <t>$ 950,33</t>
         </is>
       </c>
     </row>
@@ -10809,7 +10809,7 @@
       <c r="E371" t="inlineStr"/>
       <c r="F371" t="inlineStr">
         <is>
-          <t>$ 1.032,97</t>
+          <t>$ 950,33</t>
         </is>
       </c>
     </row>
@@ -10837,7 +10837,7 @@
       <c r="E372" t="inlineStr"/>
       <c r="F372" t="inlineStr">
         <is>
-          <t>$ 1.032,97</t>
+          <t>$ 950,33</t>
         </is>
       </c>
     </row>
@@ -10921,7 +10921,7 @@
       <c r="E375" t="inlineStr"/>
       <c r="F375" t="inlineStr">
         <is>
-          <t>$ 2.479,25</t>
+          <t>$ 2.148,68</t>
         </is>
       </c>
     </row>
@@ -11173,7 +11173,7 @@
       <c r="E384" t="inlineStr"/>
       <c r="F384" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 785,04</t>
         </is>
       </c>
     </row>
@@ -11201,7 +11201,7 @@
       <c r="E385" t="inlineStr"/>
       <c r="F385" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 785,04</t>
         </is>
       </c>
     </row>

</xml_diff>